<commit_message>
I Am Rich analysis, cleaned scripts
</commit_message>
<xml_diff>
--- a/drew charts.xlsx
+++ b/drew charts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9957243c41607423/Documents/NSS_Data_Analytics/projects/app-trader-anonymousthreat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapto\OneDrive\Documents\NSS_Data_Analytics\projects\app-trader-anonymousthreat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6ADABC29-BE22-446F-906E-F3361E96EC8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{6ADABC29-BE22-446F-906E-F3361E96EC8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ECC346B7-8B54-4932-B02D-1114AE6FE01B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query" sheetId="1" r:id="rId1"/>
@@ -20,24 +20,26 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Query!$A$1:$I$201</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">Charts!$A$40</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Charts!$A$41:$A$46</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Charts!$C$40</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Charts!$C$41:$C$46</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Charts!$F$24</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Charts!$F$25:$F$30</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Charts!$H$24</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Charts!$H$25:$H$30</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="18" r:id="rId5"/>
+    <pivotCache cacheId="8" r:id="rId5"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="261">
   <si>
     <t>app_name</t>
   </si>
@@ -757,13 +759,77 @@
   </si>
   <si>
     <t>Break Even Rating</t>
+  </si>
+  <si>
+    <t>I AM RICH PRO PLUS</t>
+  </si>
+  <si>
+    <t>I am Rich!</t>
+  </si>
+  <si>
+    <t>I am rich (Most expensive app)</t>
+  </si>
+  <si>
+    <t>I am Rich Person</t>
+  </si>
+  <si>
+    <t>I am Rich</t>
+  </si>
+  <si>
+    <t>I Am Rich</t>
+  </si>
+  <si>
+    <t>i am rich</t>
+  </si>
+  <si>
+    <t>I Am Rich Pro</t>
+  </si>
+  <si>
+    <t>I'm Rich - Trump Edition</t>
+  </si>
+  <si>
+    <t>I am rich VIP</t>
+  </si>
+  <si>
+    <t>I am rich(premium)</t>
+  </si>
+  <si>
+    <t>I am Rich Premium Plus</t>
+  </si>
+  <si>
+    <t>ðŸ’Ž I'm rich</t>
+  </si>
+  <si>
+    <t>I am Rich Plus</t>
+  </si>
+  <si>
+    <t>I AM RICH</t>
+  </si>
+  <si>
+    <t>I Am Rich Premium</t>
+  </si>
+  <si>
+    <t>I am rich</t>
+  </si>
+  <si>
+    <t>Clout</t>
+  </si>
+  <si>
+    <t>Review Count</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
@@ -1251,7 +1317,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1262,6 +1328,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1308,7 +1376,47 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -6798,7 +6906,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Drew Konig" refreshedDate="44065.409659375" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="200">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Drew Konig" refreshedDate="44065.409659375" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="200" xr:uid="{00000000-000A-0000-FFFF-FFFF12000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I201" sheet="Query"/>
   </cacheSource>
@@ -9662,7 +9770,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField dataField="1" showAll="0">
@@ -9947,7 +10055,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable4" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:C8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField showAll="0">
@@ -10625,7 +10733,7 @@
     <dataField name="App Store Reviews" fld="7" subtotal="average" baseField="3" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="3">
+    <format dxfId="7">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -10637,7 +10745,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="6">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -10650,7 +10758,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -10664,7 +10772,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="4">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -10996,7 +11104,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K201"/>
   <sheetViews>
@@ -16843,7 +16951,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I201">
+  <autoFilter ref="A1:I201" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="5">
       <filters>
         <filter val="1.99"/>
@@ -16863,7 +16971,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16938,7 +17046,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17032,21 +17140,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A40:C46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A40:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:C46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>237</v>
       </c>
@@ -17056,8 +17168,23 @@
       <c r="C40" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E40" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>1</v>
       </c>
@@ -17069,8 +17196,24 @@
         <f>(($B$41/18000)-1)/2</f>
         <v>-0.22222222222222221</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E41" s="8">
+        <v>399.99</v>
+      </c>
+      <c r="F41" t="s">
+        <v>256</v>
+      </c>
+      <c r="G41">
+        <v>3.8</v>
+      </c>
+      <c r="H41">
+        <v>3547</v>
+      </c>
+      <c r="I41" s="5">
+        <f>G41*H41</f>
+        <v>13478.599999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>5</v>
       </c>
@@ -17082,8 +17225,24 @@
         <f>(($B$42/18000)-1)/2</f>
         <v>0.88888888888888884</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E42" s="8">
+        <v>399.99</v>
+      </c>
+      <c r="F42" t="s">
+        <v>255</v>
+      </c>
+      <c r="G42">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H42">
+        <v>1867</v>
+      </c>
+      <c r="I42" s="5">
+        <f>G42*H42</f>
+        <v>7654.6999999999989</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>10</v>
       </c>
@@ -17095,8 +17254,24 @@
         <f>(($B$43/18000)-1)/2</f>
         <v>2.2777777777777777</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E43" s="8">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>254</v>
+      </c>
+      <c r="G43">
+        <v>3.9</v>
+      </c>
+      <c r="H43">
+        <v>1455</v>
+      </c>
+      <c r="I43" s="5">
+        <f>G43*H43</f>
+        <v>5674.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>15</v>
       </c>
@@ -17108,8 +17283,24 @@
         <f>(($B$44/18000)-1)/2</f>
         <v>3.666666666666667</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E44" s="8">
+        <v>399.99</v>
+      </c>
+      <c r="F44" t="s">
+        <v>253</v>
+      </c>
+      <c r="G44">
+        <v>4</v>
+      </c>
+      <c r="H44">
+        <v>856</v>
+      </c>
+      <c r="I44" s="5">
+        <f>G44*H44</f>
+        <v>3424</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>20</v>
       </c>
@@ -17121,8 +17312,24 @@
         <f>(($B$45/18000)-1)/2</f>
         <v>5.0555555555555554</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E45" s="8">
+        <v>399.99</v>
+      </c>
+      <c r="F45" t="s">
+        <v>252</v>
+      </c>
+      <c r="G45">
+        <v>3.8</v>
+      </c>
+      <c r="H45">
+        <v>718</v>
+      </c>
+      <c r="I45" s="5">
+        <f>G45*H45</f>
+        <v>2728.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>400</v>
       </c>
@@ -17134,8 +17341,286 @@
         <f>(($B$46/18000)-1)/2</f>
         <v>110.61111111111111</v>
       </c>
+      <c r="E46" s="8">
+        <v>18.989999999999998</v>
+      </c>
+      <c r="F46" t="s">
+        <v>251</v>
+      </c>
+      <c r="G46">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H46">
+        <v>459</v>
+      </c>
+      <c r="I46" s="5">
+        <f>G46*H46</f>
+        <v>2111.3999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E47" s="8">
+        <v>399.99</v>
+      </c>
+      <c r="F47" t="s">
+        <v>250</v>
+      </c>
+      <c r="G47">
+        <v>3.5</v>
+      </c>
+      <c r="H47">
+        <v>472</v>
+      </c>
+      <c r="I47" s="5">
+        <f>G47*H47</f>
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E48" s="8">
+        <v>299.99</v>
+      </c>
+      <c r="F48" t="s">
+        <v>249</v>
+      </c>
+      <c r="G48">
+        <v>3.8</v>
+      </c>
+      <c r="H48">
+        <v>411</v>
+      </c>
+      <c r="I48" s="5">
+        <f>G48*H48</f>
+        <v>1561.8</v>
+      </c>
+    </row>
+    <row r="49" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E49" s="8">
+        <v>400</v>
+      </c>
+      <c r="F49" t="s">
+        <v>248</v>
+      </c>
+      <c r="G49">
+        <v>3.6</v>
+      </c>
+      <c r="H49">
+        <v>275</v>
+      </c>
+      <c r="I49" s="5">
+        <f>G49*H49</f>
+        <v>990</v>
+      </c>
+    </row>
+    <row r="50" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E50" s="8">
+        <v>399.99</v>
+      </c>
+      <c r="F50" t="s">
+        <v>247</v>
+      </c>
+      <c r="G50">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H50">
+        <v>201</v>
+      </c>
+      <c r="I50" s="5">
+        <f>G50*H50</f>
+        <v>884.40000000000009</v>
+      </c>
+    </row>
+    <row r="51" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E51" s="8">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>246</v>
+      </c>
+      <c r="G51">
+        <v>3.9</v>
+      </c>
+      <c r="H51">
+        <v>213</v>
+      </c>
+      <c r="I51" s="5">
+        <f>G51*H51</f>
+        <v>830.69999999999993</v>
+      </c>
+    </row>
+    <row r="52" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E52" s="8">
+        <v>389.99</v>
+      </c>
+      <c r="F52" t="s">
+        <v>245</v>
+      </c>
+      <c r="G52">
+        <v>3.6</v>
+      </c>
+      <c r="H52">
+        <v>217</v>
+      </c>
+      <c r="I52" s="5">
+        <f>G52*H52</f>
+        <v>781.2</v>
+      </c>
+    </row>
+    <row r="53" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E53" s="8">
+        <v>399.99</v>
+      </c>
+      <c r="F53" t="s">
+        <v>244</v>
+      </c>
+      <c r="G53">
+        <v>4.3</v>
+      </c>
+      <c r="H53">
+        <v>180</v>
+      </c>
+      <c r="I53" s="5">
+        <f>G53*H53</f>
+        <v>774</v>
+      </c>
+    </row>
+    <row r="54" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E54" s="8">
+        <v>37.99</v>
+      </c>
+      <c r="F54" t="s">
+        <v>243</v>
+      </c>
+      <c r="G54">
+        <v>4.2</v>
+      </c>
+      <c r="H54">
+        <v>134</v>
+      </c>
+      <c r="I54" s="5">
+        <f>G54*H54</f>
+        <v>562.80000000000007</v>
+      </c>
+    </row>
+    <row r="55" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E55" s="8">
+        <v>399.99</v>
+      </c>
+      <c r="F55" t="s">
+        <v>242</v>
+      </c>
+      <c r="G55">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H55">
+        <v>129</v>
+      </c>
+      <c r="I55" s="5">
+        <f>G55*H55</f>
+        <v>528.9</v>
+      </c>
+    </row>
+    <row r="56" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E56" s="8">
+        <v>399.99</v>
+      </c>
+      <c r="F56" t="s">
+        <v>241</v>
+      </c>
+      <c r="G56">
+        <v>3.8</v>
+      </c>
+      <c r="H56">
+        <v>93</v>
+      </c>
+      <c r="I56" s="5">
+        <f>G56*H56</f>
+        <v>353.4</v>
+      </c>
+    </row>
+    <row r="57" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E57" s="8">
+        <v>399.99</v>
+      </c>
+      <c r="F57" t="s">
+        <v>240</v>
+      </c>
+      <c r="G57">
+        <v>4</v>
+      </c>
+      <c r="H57">
+        <v>36</v>
+      </c>
+      <c r="I57" s="5">
+        <f>G57*H57</f>
+        <v>144</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E41:H57">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G57">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="greaterThan">
+      <formula>4.3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G41:G57">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="greaterThan">
+      <formula>4.15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H41:H57">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41:E57">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>200</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>200</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41:I57">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>